<commit_message>
Adiona novas camadas de limites administrativos, remove camadas desatualizadas (subordinadas a rede de equipamentos), atualiza a camada de rede de equipamentos, corrije a localização da casa da mulher de caichoeirinha
</commit_message>
<xml_diff>
--- a/bases/Rede de serviços.xlsx
+++ b/bases/Rede de serviços.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="630" yWindow="585" windowWidth="22695" windowHeight="9150"/>
+  </bookViews>
   <sheets>
-    <sheet name="rede_servicos" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="rede_servicos" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="422">
   <si>
     <t>cd_identif</t>
   </si>
@@ -126,7 +130,7 @@
     <t>MULHER</t>
   </si>
   <si>
-    <t>Centro de Defesa e de Convivência da Mulher - Mulheres Vivas</t>
+    <t>Casa da Mulher Mulheres Vivas</t>
   </si>
   <si>
     <t>17</t>
@@ -150,7 +154,7 @@
     <t>270070</t>
   </si>
   <si>
-    <t>Centro de Defesa e de Convivência da Mulher - Casa Cidinha Kopcak</t>
+    <t>Casa da Mulher Cidinha Kopcak</t>
   </si>
   <si>
     <t>73</t>
@@ -177,7 +181,7 @@
     <t>270071</t>
   </si>
   <si>
-    <t>Centro de Defesa e de Convivência da Mulher - Casa Anastácia</t>
+    <t>Casa da Mulher Anastácia</t>
   </si>
   <si>
     <t>25</t>
@@ -198,7 +202,7 @@
     <t>270072</t>
   </si>
   <si>
-    <t>Centro de Defesa e de Convivência da Mulher - Marielle Franco</t>
+    <t>Casa da Mulher Marielle Franco</t>
   </si>
   <si>
     <t>GUAIANASES</t>
@@ -216,7 +220,7 @@
     <t>270073</t>
   </si>
   <si>
-    <t>Centro de Defesa e de Convivência da Mulher - Casa Marcia Martins</t>
+    <t>Casa da Mulher Marcia Martins</t>
   </si>
   <si>
     <t>Rua Cânio Rizzo, 285</t>
@@ -228,7 +232,7 @@
     <t>270074</t>
   </si>
   <si>
-    <t>Centro de Defesa e de Convivência da Mulher - Casa Viviane dos Santos</t>
+    <t>Casa da Mulher Viviane dos Santos</t>
   </si>
   <si>
     <t>96</t>
@@ -246,7 +250,7 @@
     <t>270075</t>
   </si>
   <si>
-    <t>Centro de Defesa e de Convivência da Mulher - Sônia Maria Batista</t>
+    <t>Casa da Mulher Sônia Maria Batista</t>
   </si>
   <si>
     <t>34</t>
@@ -267,7 +271,7 @@
     <t>270076</t>
   </si>
   <si>
-    <t>Centro de Defesa e de Convivência da Mulher - Casa da Mulher Crê-ser</t>
+    <t>Casa da Mulher Crê-ser</t>
   </si>
   <si>
     <t>22</t>
@@ -396,7 +400,7 @@
     <t>270082</t>
   </si>
   <si>
-    <t>Centro de Defesa e de Convivência da Mulher - Casa de Isabel Projeto Naná Serafim</t>
+    <t>Casa da Mulher Isabel Projeto Naná Serafim</t>
   </si>
   <si>
     <t>36</t>
@@ -417,7 +421,7 @@
     <t>270083</t>
   </si>
   <si>
-    <t>Centro de Defesa e de Convivência da Mulher - Casa Sofia</t>
+    <t>Casa da Mulher Sofia</t>
   </si>
   <si>
     <t>43</t>
@@ -435,7 +439,7 @@
     <t>270084</t>
   </si>
   <si>
-    <t>Centro de Defesa e de Convivência da Mulher - Centro de Integração Social da Mulher</t>
+    <t>Casa da Mulher Centro de Integração Social da Mulher</t>
   </si>
   <si>
     <t>21</t>
@@ -453,7 +457,7 @@
     <t>270085</t>
   </si>
   <si>
-    <t>Centro de Defesa e de Convivência da Mulher - Margarida Maria Alves</t>
+    <t>Casa da Mulher Margarida Maria Alves</t>
   </si>
   <si>
     <t>37</t>
@@ -507,7 +511,7 @@
     <t>270022</t>
   </si>
   <si>
-    <t>Centro de Cidadania da Mulher - Capela do Socorro</t>
+    <t>Casa da Mulher Capela do Socorro</t>
   </si>
   <si>
     <t>GRAJAU</t>
@@ -522,7 +526,7 @@
     <t>270020</t>
   </si>
   <si>
-    <t>Centro de Cidadania da Mulher - Itaquera</t>
+    <t>Casa da Mulher Itaquera</t>
   </si>
   <si>
     <t>Rua Ibiajara, 495</t>
@@ -534,7 +538,7 @@
     <t>270018</t>
   </si>
   <si>
-    <t>Centro de Cidadania da Mulher - Parelheiros</t>
+    <t>Casa da Mulher Parelheiros</t>
   </si>
   <si>
     <t>55</t>
@@ -555,7 +559,7 @@
     <t>270021</t>
   </si>
   <si>
-    <t>Centro de Cidadania da Mulher - Perus</t>
+    <t>Casa da Mulher Perus</t>
   </si>
   <si>
     <t>61</t>
@@ -573,7 +577,7 @@
     <t>270019</t>
   </si>
   <si>
-    <t>Centro de Cidadania da Mulher - Santo Amaro</t>
+    <t>Casa da Mulher  Santo Amaro</t>
   </si>
   <si>
     <t>71</t>
@@ -654,7 +658,7 @@
     <t>270038</t>
   </si>
   <si>
-    <t>Centro de Defesa e de Convivência da Mulher - Casa Mariás</t>
+    <t>Casa da Mulher Mariás</t>
   </si>
   <si>
     <t>89</t>
@@ -672,7 +676,7 @@
     <t>270039</t>
   </si>
   <si>
-    <t>Centro de Defesa e de Convivência da Mulher - Casa Zizi</t>
+    <t>Casa da Mulher Zizi</t>
   </si>
   <si>
     <t>72</t>
@@ -696,7 +700,7 @@
     <t>270040</t>
   </si>
   <si>
-    <t>Centro de Defesa e de Convivência da Mulher - Espaço Francisca Franco</t>
+    <t>Casa da Mulher Espaço Francisca Franco</t>
   </si>
   <si>
     <t>Rua Conselheiro Ramalho, 93</t>
@@ -852,7 +856,7 @@
     <t>270014</t>
   </si>
   <si>
-    <t>Centro de Referência e Cidadania da Mulher - Casa da Mulher 25 de Março</t>
+    <t>Casa da Mulher 25 de Março</t>
   </si>
   <si>
     <t>BARRA FUNDA</t>
@@ -867,7 +871,7 @@
     <t>270017</t>
   </si>
   <si>
-    <t>Centro de Referência e Cidadania da Mulher - Casa da Mulher de Brasilândia</t>
+    <t>Casa da Mulher  Brasilândia</t>
   </si>
   <si>
     <t>Rua Sílvio Bueno Peruche, 538</t>
@@ -879,13 +883,19 @@
     <t>270048</t>
   </si>
   <si>
-    <t>Centro de Referência e Cidadania da Mulher - Casa da Mulher de Cachoeirinha</t>
+    <t>Casa da Mulher Cachoeirinha</t>
+  </si>
+  <si>
+    <t>Avenida Deputado Emílio Carlos, 3460</t>
+  </si>
+  <si>
+    <t>02721-200</t>
   </si>
   <si>
     <t>270049</t>
   </si>
   <si>
-    <t>Centro de Referência e Cidadania da Mulher - Casa da Mulher de Săo Miguel</t>
+    <t>Casa da Mulher Săo Miguel</t>
   </si>
   <si>
     <t>Rua Pedro Soares de Andrade, 34</t>
@@ -897,7 +907,7 @@
     <t>270016</t>
   </si>
   <si>
-    <t>Centro de Referência e Cidadania da Mulher - Casa da Mulher Eliane de Grammont</t>
+    <t>Casa da Mulher Eliane de Grammont</t>
   </si>
   <si>
     <t>90</t>
@@ -915,7 +925,7 @@
     <t>270015</t>
   </si>
   <si>
-    <t>Centro de Referência e Cidadania da Mulher - Casa da Mulher Maria de Lourdes Rodrigues</t>
+    <t>Casa da Mulher Maria de Lourdes Rodrigues</t>
   </si>
   <si>
     <t>Rua Raphaela Miraglia Scoppetta, 50</t>
@@ -1275,29 +1285,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="DD/MM/YY" numFmtId="165"/>
-    <numFmt formatCode="DD/MM/YYYY\ HH:MM:SS" numFmtId="166"/>
-    <numFmt formatCode="HH:MM:SS" numFmtId="167"/>
-    <numFmt formatCode="DD/MM/YYYY\ HH:MM:SS.000" numFmtId="168"/>
-    <numFmt formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;" numFmtId="169"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <sz val="10"/>
     </font>
   </fonts>
-  <fills count="1">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
+    <fill>
+      <patternFill patternType="gray125"/>
+    </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1306,43 +1311,321 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="164">
-</xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="164" xfId="0"/>
-    <xf numFmtId="165" xfId="0"/>
-    <xf numFmtId="166" xfId="0"/>
-    <xf numFmtId="167" xfId="0"/>
-    <xf numFmtId="168" xfId="0"/>
-    <xf numFmtId="169" xfId="0"/>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+  <a:themeElements>
+    <a:clrScheme name="Escritório">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Escritório">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Escritório">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N73"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1024" width="15"/>
-    <col min="2" max="1024" width="15"/>
-    <col min="3" max="1024" width="15"/>
-    <col min="4" max="1024" width="15"/>
-    <col min="5" max="1024" width="15"/>
-    <col min="6" max="1024" width="15"/>
-    <col min="7" max="1024" width="15"/>
-    <col min="8" max="1024" width="15"/>
-    <col min="9" max="1024" width="15"/>
-    <col min="10" max="1024" width="15"/>
-    <col min="11" max="1024" width="15"/>
-    <col min="12" max="1024" width="15"/>
-    <col min="13" max="1024" width="15"/>
-    <col min="14" max="1024" width="15"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1386,7 +1669,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1424,13 +1707,13 @@
         <v>24</v>
       </c>
       <c r="M2">
-        <v>-23.55321078996814</v>
+        <v>-23.553210789968141</v>
       </c>
       <c r="N2">
-        <v>-46.6393532538675</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>-46.639353253867498</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1468,13 +1751,13 @@
         <v>34</v>
       </c>
       <c r="M3">
-        <v>-23.58822606962702</v>
+        <v>-23.588226069627019</v>
       </c>
       <c r="N3">
-        <v>-46.73017242925276</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>-46.730172429252761</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -1512,13 +1795,13 @@
         <v>44</v>
       </c>
       <c r="M4">
-        <v>-23.63409060468359</v>
+        <v>-23.634090604683589</v>
       </c>
       <c r="N4">
-        <v>-46.77171251509468</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>-46.771712515094677</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -1556,13 +1839,13 @@
         <v>53</v>
       </c>
       <c r="M5">
-        <v>-23.60144560769031</v>
+        <v>-23.601445607690309</v>
       </c>
       <c r="N5">
-        <v>-46.48215516310255</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>-46.482155163102547</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -1603,10 +1886,10 @@
         <v>-23.57995366455939</v>
       </c>
       <c r="N6">
-        <v>-46.41277620717857</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>-46.412776207178567</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>61</v>
       </c>
@@ -1644,13 +1927,13 @@
         <v>66</v>
       </c>
       <c r="M7">
-        <v>-23.55561780814593</v>
+        <v>-23.555617808145929</v>
       </c>
       <c r="N7">
-        <v>-46.41367186312422</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>-46.413671863124222</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -1688,13 +1971,13 @@
         <v>70</v>
       </c>
       <c r="M8">
-        <v>-23.58831872234463</v>
+        <v>-23.588318722344631</v>
       </c>
       <c r="N8">
-        <v>-46.73177610421126</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>-46.731776104211256</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>71</v>
       </c>
@@ -1735,10 +2018,10 @@
         <v>-23.53529210199671</v>
       </c>
       <c r="N9">
-        <v>-46.40102076462913</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>-46.401020764629131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>77</v>
       </c>
@@ -1776,13 +2059,13 @@
         <v>83</v>
       </c>
       <c r="M10">
-        <v>-23.60232727876284</v>
+        <v>-23.602327278762839</v>
       </c>
       <c r="N10">
-        <v>-46.60902327477665</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>-46.609023274776654</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>84</v>
       </c>
@@ -1820,13 +2103,13 @@
         <v>90</v>
       </c>
       <c r="M11">
-        <v>-23.6703983977113</v>
+        <v>-23.670398397711299</v>
       </c>
       <c r="N11">
-        <v>-46.66357963603127</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>-46.663579636031272</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>91</v>
       </c>
@@ -1864,13 +2147,13 @@
         <v>97</v>
       </c>
       <c r="M12">
-        <v>-23.49568406388003</v>
+        <v>-23.495684063880031</v>
       </c>
       <c r="N12">
-        <v>-46.44307713366241</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>-46.443077133662413</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>98</v>
       </c>
@@ -1908,13 +2191,13 @@
         <v>104</v>
       </c>
       <c r="M13">
-        <v>-23.50078727882907</v>
+        <v>-23.500787278829069</v>
       </c>
       <c r="N13">
         <v>-46.61335063366127</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>105</v>
       </c>
@@ -1952,13 +2235,13 @@
         <v>111</v>
       </c>
       <c r="M14">
-        <v>-23.74210099246937</v>
+        <v>-23.742100992469371</v>
       </c>
       <c r="N14">
-        <v>-46.71015603365338</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>-46.710156033653377</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>112</v>
       </c>
@@ -1996,13 +2279,13 @@
         <v>119</v>
       </c>
       <c r="M15">
-        <v>-23.6500241217798</v>
+        <v>-23.650024121779801</v>
       </c>
       <c r="N15">
-        <v>-46.74880082200398</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>-46.748800822003979</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>120</v>
       </c>
@@ -2043,10 +2326,10 @@
         <v>-23.47427913907644</v>
       </c>
       <c r="N16">
-        <v>-46.65321854532546</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>-46.653218545325458</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>127</v>
       </c>
@@ -2087,10 +2370,10 @@
         <v>-23.50240607882829</v>
       </c>
       <c r="N17">
-        <v>-46.39447068641498</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>-46.394470686414977</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>134</v>
       </c>
@@ -2128,13 +2411,13 @@
         <v>139</v>
       </c>
       <c r="M18">
-        <v>-23.68339836463045</v>
+        <v>-23.683398364630449</v>
       </c>
       <c r="N18">
-        <v>-46.76803704531224</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>-46.768037045312241</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>140</v>
       </c>
@@ -2172,13 +2455,13 @@
         <v>145</v>
       </c>
       <c r="M19">
-        <v>-23.50846295594715</v>
+        <v>-23.508462955947149</v>
       </c>
       <c r="N19">
-        <v>-46.66699799970709</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>-46.666997999707093</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>146</v>
       </c>
@@ -2216,13 +2499,13 @@
         <v>152</v>
       </c>
       <c r="M20">
-        <v>-23.55056086499974</v>
+        <v>-23.550560864999738</v>
       </c>
       <c r="N20">
-        <v>-46.44467127802967</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>-46.444671278029674</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>153</v>
       </c>
@@ -2263,10 +2546,10 @@
         <v>-23.55945452276972</v>
       </c>
       <c r="N21">
-        <v>-46.62446097476438</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>-46.624460974764382</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>160</v>
       </c>
@@ -2304,13 +2587,13 @@
         <v>163</v>
       </c>
       <c r="M22">
-        <v>-23.55741497186967</v>
+        <v>-23.557414971869669</v>
       </c>
       <c r="N22">
-        <v>-46.62287759797812</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>-46.622877597978118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>164</v>
       </c>
@@ -2351,10 +2634,10 @@
         <v>-23.7352576963297</v>
       </c>
       <c r="N23">
-        <v>-46.69110374646446</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>-46.691103746464456</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>169</v>
       </c>
@@ -2392,13 +2675,13 @@
         <v>172</v>
       </c>
       <c r="M24">
-        <v>-23.52992526973397</v>
+        <v>-23.529925269733969</v>
       </c>
       <c r="N24">
-        <v>-46.4349929497199</v>
-      </c>
-    </row>
-    <row r="25">
+        <v>-46.434992949719899</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>173</v>
       </c>
@@ -2436,13 +2719,13 @@
         <v>179</v>
       </c>
       <c r="M25">
-        <v>-23.82793578755401</v>
+        <v>-23.827935787554011</v>
       </c>
       <c r="N25">
-        <v>-46.72268354103141</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>-46.722683541031408</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>180</v>
       </c>
@@ -2483,10 +2766,10 @@
         <v>-23.41522002257209</v>
       </c>
       <c r="N26">
-        <v>-46.75357373377251</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>-46.753573733772512</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>186</v>
       </c>
@@ -2527,10 +2810,10 @@
         <v>-23.65044914315316</v>
       </c>
       <c r="N27">
-        <v>-46.70801870538986</v>
-      </c>
-    </row>
-    <row r="28">
+        <v>-46.708018705389861</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>192</v>
       </c>
@@ -2568,13 +2851,13 @@
         <v>200</v>
       </c>
       <c r="M28">
-        <v>-23.53372410784315</v>
+        <v>-23.533724107843149</v>
       </c>
       <c r="N28">
-        <v>-46.7062525088233</v>
-      </c>
-    </row>
-    <row r="29">
+        <v>-46.706252508823297</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>201</v>
       </c>
@@ -2612,13 +2895,13 @@
         <v>204</v>
       </c>
       <c r="M29">
-        <v>-23.6490737048774</v>
+        <v>-23.649073704877399</v>
       </c>
       <c r="N29">
-        <v>-46.69908437873127</v>
-      </c>
-    </row>
-    <row r="30">
+        <v>-46.699084378731271</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>205</v>
       </c>
@@ -2659,10 +2942,10 @@
         <v>-23.49760268971308</v>
       </c>
       <c r="N30">
-        <v>-46.4414310533412</v>
-      </c>
-    </row>
-    <row r="31">
+        <v>-46.441431053341198</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>209</v>
       </c>
@@ -2703,10 +2986,10 @@
         <v>-23.50963403966087</v>
       </c>
       <c r="N31">
-        <v>-46.65761682214197</v>
-      </c>
-    </row>
-    <row r="32">
+        <v>-46.657616822141968</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>213</v>
       </c>
@@ -2744,13 +3027,13 @@
         <v>218</v>
       </c>
       <c r="M32">
-        <v>-23.5062363005246</v>
+        <v>-23.506236300524598</v>
       </c>
       <c r="N32">
-        <v>-46.57621921764986</v>
-      </c>
-    </row>
-    <row r="33">
+        <v>-46.576219217649857</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>219</v>
       </c>
@@ -2788,13 +3071,13 @@
         <v>226</v>
       </c>
       <c r="M33">
-        <v>-23.58651119609928</v>
+        <v>-23.586511196099281</v>
       </c>
       <c r="N33">
-        <v>-46.54366043113959</v>
-      </c>
-    </row>
-    <row r="34">
+        <v>-46.543660431139593</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>227</v>
       </c>
@@ -2835,10 +3118,10 @@
         <v>-23.55238161257158</v>
       </c>
       <c r="N34">
-        <v>-46.64480095997643</v>
-      </c>
-    </row>
-    <row r="35">
+        <v>-46.644800959976429</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>231</v>
       </c>
@@ -2879,10 +3162,10 @@
         <v>-23.53378179301739</v>
       </c>
       <c r="N35">
-        <v>-46.63075572494534</v>
-      </c>
-    </row>
-    <row r="36">
+        <v>-46.630755724945338</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>237</v>
       </c>
@@ -2923,10 +3206,10 @@
         <v>-23.56097702209901</v>
       </c>
       <c r="N36">
-        <v>-46.6404743115863</v>
-      </c>
-    </row>
-    <row r="37">
+        <v>-46.640474311586303</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>242</v>
       </c>
@@ -2964,13 +3247,13 @@
         <v>245</v>
       </c>
       <c r="M37">
-        <v>-23.5843045413036</v>
+        <v>-23.584304541303599</v>
       </c>
       <c r="N37">
-        <v>-46.40872181572746</v>
-      </c>
-    </row>
-    <row r="38">
+        <v>-46.408721815727461</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>246</v>
       </c>
@@ -3011,10 +3294,10 @@
         <v>-23.4976619481046</v>
       </c>
       <c r="N38">
-        <v>-46.40165990326413</v>
-      </c>
-    </row>
-    <row r="39">
+        <v>-46.401659903264132</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>250</v>
       </c>
@@ -3058,7 +3341,7 @@
         <v>-46.60061337210113</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>254</v>
       </c>
@@ -3099,10 +3382,10 @@
         <v>-23.45256237483521</v>
       </c>
       <c r="N40">
-        <v>-46.67480223013924</v>
-      </c>
-    </row>
-    <row r="41">
+        <v>-46.674802230139242</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>261</v>
       </c>
@@ -3143,10 +3426,10 @@
         <v>-23.58702458640083</v>
       </c>
       <c r="N41">
-        <v>-46.73280621152455</v>
-      </c>
-    </row>
-    <row r="42">
+        <v>-46.732806211524547</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>266</v>
       </c>
@@ -3184,13 +3467,13 @@
         <v>269</v>
       </c>
       <c r="M42">
-        <v>-23.63312362358081</v>
+        <v>-23.633123623580811</v>
       </c>
       <c r="N42">
-        <v>-46.77631971602958</v>
-      </c>
-    </row>
-    <row r="43">
+        <v>-46.776319716029583</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>270</v>
       </c>
@@ -3231,10 +3514,10 @@
         <v>-23.81509707870422</v>
       </c>
       <c r="N43">
-        <v>-46.73576621429883</v>
-      </c>
-    </row>
-    <row r="44">
+        <v>-46.735766214298827</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>274</v>
       </c>
@@ -3272,13 +3555,13 @@
         <v>278</v>
       </c>
       <c r="M44">
-        <v>-23.55862056568119</v>
+        <v>-23.558620565681188</v>
       </c>
       <c r="N44">
-        <v>-46.6427634351095</v>
-      </c>
-    </row>
-    <row r="45">
+        <v>-46.642763435109501</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>279</v>
       </c>
@@ -3316,13 +3599,13 @@
         <v>283</v>
       </c>
       <c r="M45">
-        <v>-23.52962256766949</v>
+        <v>-23.529622567669492</v>
       </c>
       <c r="N45">
-        <v>-46.67265400952334</v>
-      </c>
-    </row>
-    <row r="46">
+        <v>-46.672654009523342</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>284</v>
       </c>
@@ -3363,10 +3646,10 @@
         <v>-23.46329429684398</v>
       </c>
       <c r="N46">
-        <v>-46.67835126379848</v>
-      </c>
-    </row>
-    <row r="47">
+        <v>-46.678351263798483</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>288</v>
       </c>
@@ -3398,21 +3681,21 @@
         <v>32</v>
       </c>
       <c r="K47" t="s">
-        <v>144</v>
+        <v>290</v>
       </c>
       <c r="L47" t="s">
-        <v>145</v>
+        <v>291</v>
       </c>
       <c r="M47">
-        <v>-23.50821591972507</v>
+        <v>-23.477804053634369</v>
       </c>
       <c r="N47">
-        <v>-46.66700843114113</v>
-      </c>
-    </row>
-    <row r="48">
+        <v>-46.671271274611691</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B48" t="s">
         <v>36</v>
@@ -3421,7 +3704,7 @@
         <v>37</v>
       </c>
       <c r="D48" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="E48" t="s">
         <v>93</v>
@@ -3442,21 +3725,21 @@
         <v>51</v>
       </c>
       <c r="K48" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="L48" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="M48">
         <v>-23.49511903795813</v>
       </c>
       <c r="N48">
-        <v>-46.43663243141847</v>
-      </c>
-    </row>
-    <row r="49">
+        <v>-46.436632431418467</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="B49" t="s">
         <v>36</v>
@@ -3465,19 +3748,19 @@
         <v>37</v>
       </c>
       <c r="D49" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="E49" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="F49" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="G49" t="s">
         <v>263</v>
       </c>
       <c r="H49" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="I49" t="s">
         <v>41</v>
@@ -3486,21 +3769,21 @@
         <v>42</v>
       </c>
       <c r="K49" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="L49" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="M49">
-        <v>-23.59439299351702</v>
+        <v>-23.594392993517019</v>
       </c>
       <c r="N49">
-        <v>-46.64771821594304</v>
-      </c>
-    </row>
-    <row r="50">
+        <v>-46.647718215943037</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B50" t="s">
         <v>36</v>
@@ -3509,7 +3792,7 @@
         <v>37</v>
       </c>
       <c r="D50" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="E50" t="s">
         <v>39</v>
@@ -3530,21 +3813,21 @@
         <v>42</v>
       </c>
       <c r="K50" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="L50" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="M50">
-        <v>-23.65039605048223</v>
+        <v>-23.650396050482229</v>
       </c>
       <c r="N50">
-        <v>-46.75969544369669</v>
-      </c>
-    </row>
-    <row r="51">
+        <v>-46.759695443696693</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="B51" t="s">
         <v>31</v>
@@ -3553,13 +3836,13 @@
         <v>193</v>
       </c>
       <c r="D51" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="E51" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="F51" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="G51" t="s">
         <v>20</v>
@@ -3574,30 +3857,30 @@
         <v>22</v>
       </c>
       <c r="K51" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="L51" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="M51">
-        <v>-23.54534288105989</v>
+        <v>-23.545342881059891</v>
       </c>
       <c r="N51">
-        <v>-46.64692882929346</v>
-      </c>
-    </row>
-    <row r="52">
+        <v>-46.646928829293458</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B52" t="s">
         <v>197</v>
       </c>
       <c r="C52" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="D52" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="E52" t="s">
         <v>18</v>
@@ -3618,30 +3901,30 @@
         <v>22</v>
       </c>
       <c r="K52" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="L52" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="M52">
-        <v>-23.54988885881317</v>
+        <v>-23.549888858813169</v>
       </c>
       <c r="N52">
-        <v>-46.63156851397766</v>
-      </c>
-    </row>
-    <row r="53">
+        <v>-46.631568513977662</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B53" t="s">
         <v>41</v>
       </c>
       <c r="C53" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D53" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="E53" t="s">
         <v>18</v>
@@ -3662,30 +3945,30 @@
         <v>22</v>
       </c>
       <c r="K53" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="L53" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="M53">
         <v>-23.54826586390708</v>
       </c>
       <c r="N53">
-        <v>-46.63766957918636</v>
-      </c>
-    </row>
-    <row r="54">
+        <v>-46.637669579186358</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="B54" t="s">
         <v>41</v>
       </c>
       <c r="C54" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D54" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="E54" t="s">
         <v>27</v>
@@ -3706,36 +3989,36 @@
         <v>198</v>
       </c>
       <c r="K54" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="L54" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="M54">
         <v>-23.58838795135593</v>
       </c>
       <c r="N54">
-        <v>-46.73806494797341</v>
-      </c>
-    </row>
-    <row r="55">
+        <v>-46.738064947973413</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B55" t="s">
         <v>41</v>
       </c>
       <c r="C55" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D55" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="E55" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="F55" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="G55" t="s">
         <v>39</v>
@@ -3750,36 +4033,36 @@
         <v>42</v>
       </c>
       <c r="K55" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="L55" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="M55">
-        <v>-23.64270694203197</v>
+        <v>-23.642706942031971</v>
       </c>
       <c r="N55">
-        <v>-46.73572121751262</v>
-      </c>
-    </row>
-    <row r="56">
+        <v>-46.735721217512619</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="B56" t="s">
         <v>41</v>
       </c>
       <c r="C56" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D56" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="E56" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="F56" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="G56" t="s">
         <v>108</v>
@@ -3794,30 +4077,30 @@
         <v>42</v>
       </c>
       <c r="K56" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="L56" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="M56">
-        <v>-23.72061458197862</v>
+        <v>-23.720614581978619</v>
       </c>
       <c r="N56">
-        <v>-46.70181183851702</v>
-      </c>
-    </row>
-    <row r="57">
+        <v>-46.701811838517017</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B57" t="s">
         <v>41</v>
       </c>
       <c r="C57" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D57" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="E57" t="s">
         <v>56</v>
@@ -3838,36 +4121,36 @@
         <v>51</v>
       </c>
       <c r="K57" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="L57" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="M57">
         <v>-23.58334945676031</v>
       </c>
       <c r="N57">
-        <v>-46.41580824622203</v>
-      </c>
-    </row>
-    <row r="58">
+        <v>-46.415808246222028</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="B58" t="s">
         <v>41</v>
       </c>
       <c r="C58" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D58" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="E58" t="s">
         <v>150</v>
       </c>
       <c r="F58" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="G58" t="s">
         <v>81</v>
@@ -3882,42 +4165,42 @@
         <v>42</v>
       </c>
       <c r="K58" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="L58" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="M58">
-        <v>-23.59760650213475</v>
+        <v>-23.597606502134749</v>
       </c>
       <c r="N58">
-        <v>-46.62177501142482</v>
-      </c>
-    </row>
-    <row r="59">
+        <v>-46.621775011424823</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B59" t="s">
         <v>41</v>
       </c>
       <c r="C59" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D59" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="E59" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="F59" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="G59" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="H59" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="I59" t="s">
         <v>41</v>
@@ -3926,30 +4209,30 @@
         <v>42</v>
       </c>
       <c r="K59" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="L59" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="M59">
         <v>-23.64787487939299</v>
       </c>
       <c r="N59">
-        <v>-46.64037867090681</v>
-      </c>
-    </row>
-    <row r="60">
+        <v>-46.640378670906813</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="B60" t="s">
         <v>41</v>
       </c>
       <c r="C60" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D60" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="E60" t="s">
         <v>195</v>
@@ -3970,42 +4253,42 @@
         <v>198</v>
       </c>
       <c r="K60" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="L60" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="M60">
-        <v>-23.52219987894732</v>
+        <v>-23.522199878947319</v>
       </c>
       <c r="N60">
-        <v>-46.69576316441798</v>
-      </c>
-    </row>
-    <row r="61">
+        <v>-46.695763164417983</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B61" t="s">
         <v>41</v>
       </c>
       <c r="C61" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D61" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="E61" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="F61" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="G61" t="s">
         <v>142</v>
       </c>
       <c r="H61" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="I61" t="s">
         <v>50</v>
@@ -4014,42 +4297,42 @@
         <v>51</v>
       </c>
       <c r="K61" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="L61" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="M61">
-        <v>-23.5186544769799</v>
+        <v>-23.518654476979901</v>
       </c>
       <c r="N61">
-        <v>-46.52103911484932</v>
-      </c>
-    </row>
-    <row r="62">
+        <v>-46.521039114849323</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="B62" t="s">
         <v>41</v>
       </c>
       <c r="C62" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D62" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="E62" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="F62" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="G62" t="s">
         <v>41</v>
       </c>
       <c r="H62" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="I62" t="s">
         <v>31</v>
@@ -4058,30 +4341,30 @@
         <v>32</v>
       </c>
       <c r="K62" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="L62" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="M62">
         <v>-23.48143288842666</v>
       </c>
       <c r="N62">
-        <v>-46.60435874140582</v>
-      </c>
-    </row>
-    <row r="63">
+        <v>-46.604358741405818</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="B63" t="s">
         <v>41</v>
       </c>
       <c r="C63" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D63" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="E63" t="s">
         <v>47</v>
@@ -4102,36 +4385,36 @@
         <v>51</v>
       </c>
       <c r="K63" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="L63" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="M63">
-        <v>-23.59992925436365</v>
+        <v>-23.599929254363651</v>
       </c>
       <c r="N63">
-        <v>-46.46950324690918</v>
-      </c>
-    </row>
-    <row r="64">
+        <v>-46.469503246909177</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="B64" t="s">
         <v>41</v>
       </c>
       <c r="C64" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D64" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="E64" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="F64" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="G64" t="s">
         <v>95</v>
@@ -4146,21 +4429,21 @@
         <v>51</v>
       </c>
       <c r="K64" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="L64" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="M64">
-        <v>-23.50054770270408</v>
+        <v>-23.500547702704079</v>
       </c>
       <c r="N64">
-        <v>-46.45132222649973</v>
-      </c>
-    </row>
-    <row r="65">
+        <v>-46.451322226499727</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B65" t="s">
         <v>123</v>
@@ -4169,7 +4452,7 @@
         <v>154</v>
       </c>
       <c r="D65" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="E65" t="s">
         <v>156</v>
@@ -4196,15 +4479,15 @@
         <v>159</v>
       </c>
       <c r="M65">
-        <v>-23.55944133330012</v>
+        <v>-23.559441333300121</v>
       </c>
       <c r="N65">
-        <v>-46.62445396974591</v>
-      </c>
-    </row>
-    <row r="66">
+        <v>-46.624453969745908</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="B66" t="s">
         <v>36</v>
@@ -4213,7 +4496,7 @@
         <v>37</v>
       </c>
       <c r="D66" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="E66" t="s">
         <v>20</v>
@@ -4234,21 +4517,21 @@
         <v>22</v>
       </c>
       <c r="K66" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="L66" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="M66">
-        <v>-23.53514760902146</v>
+        <v>-23.535147609021461</v>
       </c>
       <c r="N66">
-        <v>-46.63537633344948</v>
-      </c>
-    </row>
-    <row r="67">
+        <v>-46.635376333449479</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="B67" t="s">
         <v>36</v>
@@ -4257,7 +4540,7 @@
         <v>37</v>
       </c>
       <c r="D67" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="E67" t="s">
         <v>79</v>
@@ -4278,21 +4561,21 @@
         <v>42</v>
       </c>
       <c r="K67" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="L67" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="M67">
-        <v>-23.60293635468961</v>
+        <v>-23.602936354689611</v>
       </c>
       <c r="N67">
-        <v>-46.60253865136277</v>
-      </c>
-    </row>
-    <row r="68">
+        <v>-46.602538651362771</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="B68" t="s">
         <v>36</v>
@@ -4301,13 +4584,13 @@
         <v>37</v>
       </c>
       <c r="D68" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="E68" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="F68" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="G68" t="s">
         <v>20</v>
@@ -4322,21 +4605,21 @@
         <v>22</v>
       </c>
       <c r="K68" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="L68" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="M68">
         <v>-23.53916608926782</v>
       </c>
       <c r="N68">
-        <v>-46.6493340816579</v>
-      </c>
-    </row>
-    <row r="69">
+        <v>-46.649334081657898</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="B69" t="s">
         <v>123</v>
@@ -4345,19 +4628,19 @@
         <v>154</v>
       </c>
       <c r="D69" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="E69" t="s">
         <v>50</v>
       </c>
       <c r="F69" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="G69" t="s">
         <v>256</v>
       </c>
       <c r="H69" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="I69" t="s">
         <v>123</v>
@@ -4366,36 +4649,36 @@
         <v>198</v>
       </c>
       <c r="K69" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="L69" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="M69">
         <v>-23.53853861308945</v>
       </c>
       <c r="N69">
-        <v>-46.70831584614503</v>
-      </c>
-    </row>
-    <row r="70">
+        <v>-46.708315846145027</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B70" t="s">
         <v>21</v>
       </c>
       <c r="C70" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="D70" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="E70" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="F70" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="G70" t="s">
         <v>20</v>
@@ -4410,30 +4693,30 @@
         <v>22</v>
       </c>
       <c r="K70" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="L70" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="M70">
-        <v>-23.53515419953362</v>
+        <v>-23.535154199533618</v>
       </c>
       <c r="N70">
-        <v>-46.64014577553652</v>
-      </c>
-    </row>
-    <row r="71">
+        <v>-46.640145775536517</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="B71" t="s">
         <v>197</v>
       </c>
       <c r="C71" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="D71" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="E71" t="s">
         <v>20</v>
@@ -4454,30 +4737,30 @@
         <v>22</v>
       </c>
       <c r="K71" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="L71" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="M71">
-        <v>-23.53572279723158</v>
+        <v>-23.535722797231578</v>
       </c>
       <c r="N71">
-        <v>-46.63068251860506</v>
-      </c>
-    </row>
-    <row r="72">
+        <v>-46.630682518605063</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="B72" t="s">
         <v>21</v>
       </c>
       <c r="C72" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="D72" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="E72" t="s">
         <v>18</v>
@@ -4498,36 +4781,36 @@
         <v>22</v>
       </c>
       <c r="K72" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="L72" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="M72">
-        <v>-23.54838872738553</v>
+        <v>-23.548388727385529</v>
       </c>
       <c r="N72">
         <v>-46.63745368955847</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:14" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="B73" t="s">
         <v>197</v>
       </c>
       <c r="C73" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="D73" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="E73" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="F73" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="G73" t="s">
         <v>20</v>
@@ -4542,18 +4825,19 @@
         <v>22</v>
       </c>
       <c r="K73" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="L73" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="M73">
-        <v>-23.55867294379378</v>
+        <v>-23.558672943793781</v>
       </c>
       <c r="N73">
-        <v>-46.62798742490885</v>
+        <v>-46.627987424908852</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>